<commit_message>
Renomear planilha recem criada
Função para renomear CSV recem criado, o nome sera o grupo e a data de download do csv
</commit_message>
<xml_diff>
--- a/grupo.xlsx
+++ b/grupo.xlsx
@@ -14,12 +14,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>GRUPOS:</t>
   </si>
   <si>
     <t>ARTIGOS DE HIGIENE</t>
+  </si>
+  <si>
+    <t>DIVERSOS</t>
+  </si>
+  <si>
+    <t>EQUIPAMENTOS E ARTIGOS PARA USO MÉDICO, DENTÁRIO E VETERINÁRIO</t>
+  </si>
+  <si>
+    <t>INSTRUMENTOS E EQUIPAMENTOS DE LABORATÓRIO</t>
+  </si>
+  <si>
+    <t>MATERIAIS MANUFATURADOS, NÃO METÁLICOS</t>
+  </si>
+  <si>
+    <t>SUBSISTÊNCIA</t>
+  </si>
+  <si>
+    <t>SUBSTÂNCIAS E PRODUTOS QUÍMICOS</t>
   </si>
 </sst>
 </file>
@@ -366,7 +384,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -385,6 +403,36 @@
         <v>1</v>
       </c>
     </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>